<commit_message>
auth & profiles fixed
</commit_message>
<xml_diff>
--- a/palette-connection-service/src/data/SFModels.xlsx
+++ b/palette-connection-service/src/data/SFModels.xlsx
@@ -71,22 +71,34 @@
       <style:table-cell-properties fo:wrap-option="wrap"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Ubuntu" fo:font-size="12pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="DejaVu Sans" style:font-size-asian="12pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="DejaVu Sans" style:font-size-complex="12pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
     </style:style>
+    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:wrap-option="wrap"/>
+      <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Ubuntu" fo:font-size="14pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="DejaVu Sans" style:font-size-asian="14pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="DejaVu Sans" style:font-size-complex="14pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="bold" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:wrap-option="wrap"/>
+      <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Ubuntu" fo:font-size="14pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="DejaVu Sans" style:font-size-asian="14pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="DejaVu Sans" style:font-size-complex="14pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="ce6" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:wrap-option="wrap"/>
+      <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Ubuntu" fo:font-size="12pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="DejaVu Sans" style:font-size-asian="12pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="DejaVu Sans" style:font-size-complex="12pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
       <table:calculation-settings table:automatic-find-labels="false" table:use-regular-expressions="false" table:use-wildcards="true"/>
       <table:table table:name="TAWS" table:style-name="ta1">
-        <table:table-column table:style-name="co1" table:default-cell-style-name="ce8"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="ce8"/>
-        <table:table-column table:style-name="co3" table:default-cell-style-name="ce8"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="ce5"/>
+        <table:table-column table:style-name="co2" table:default-cell-style-name="ce5"/>
+        <table:table-column table:style-name="co3" table:default-cell-style-name="ce5"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>crmId</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>objectGlobalKeyname</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>objectCrmKeyname</text:p>
           </table:table-cell>
         </table:table-row>
@@ -318,21 +330,21 @@
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce9" table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="ce6" table:number-columns-repeated="3"/>
         </table:table-row>
       </table:table>
       <table:table table:name="Big_Thought" table:style-name="ta1">
-        <table:table-column table:style-name="co5" table:default-cell-style-name="ce8"/>
-        <table:table-column table:style-name="co6" table:default-cell-style-name="ce8"/>
-        <table:table-column table:style-name="co7" table:default-cell-style-name="ce8"/>
+        <table:table-column table:style-name="co5" table:default-cell-style-name="ce5"/>
+        <table:table-column table:style-name="co6" table:default-cell-style-name="ce5"/>
+        <table:table-column table:style-name="co7" table:default-cell-style-name="ce5"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>crmId</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>objectGlobalKeyname</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>objectCrmKeyname</text:p>
           </table:table-cell>
         </table:table-row>
@@ -467,7 +479,7 @@
             <text:p>Palette_To_Do</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Palette_Resource_Connection__c</text:p>
+            <text:p>Palette_To_Do__c</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro2">
@@ -553,7 +565,7 @@
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce9" table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="ce6" table:number-columns-repeated="3"/>
         </table:table-row>
       </table:table>
       <table:named-expressions/>
@@ -566,9 +578,9 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.2">
   <office:meta>
     <meta:creation-date>2022-02-10T09:48:23.501898960</meta:creation-date>
-    <dc:date>2022-04-23T15:18:33.527520224</dc:date>
-    <meta:editing-duration>PT5H40M23S</meta:editing-duration>
-    <meta:editing-cycles>20</meta:editing-cycles>
+    <dc:date>2022-04-24T16:06:30.488426750</dc:date>
+    <meta:editing-duration>PT5H41M2S</meta:editing-duration>
+    <meta:editing-cycles>21</meta:editing-cycles>
     <meta:generator>LibreOffice/6.4.7.2$Linux_X86_64 LibreOffice_project/40$Build-2</meta:generator>
     <meta:document-statistic meta:table-count="2" meta:cell-count="135" meta:object-count="0"/>
   </office:meta>
@@ -581,15 +593,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">20630</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">27252</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">22008</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">26042</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Big_Thought">
               <config:config-item config:name="CursorPositionX" config:type="int">2</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">13</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -662,7 +674,7 @@
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">nwH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpEdXBsZXg6Tm9uZQBQYWdlU2l6ZTpBNAAAEgBDT01QQVRfRFVQTEVYX01PREUPAER1cGxleE1vZGU6Ok9mZg==</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">nwH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpBNABEdXBsZXg6Tm9uZQAAEgBDT01QQVRfRFVQTEVYX01PREUPAER1cGxleE1vZGU6Ok9mZg==</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
@@ -829,9 +841,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2022-04-23">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2022-04-24">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="15:18:13.815605676">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="16:05:50.985545125">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>